<commit_message>
alleen nog overlap en time constraints astar
</commit_message>
<xml_diff>
--- a/Instances/T_EGS-r.xlsx
+++ b/Instances/T_EGS-r.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07ed5a09c14e9223/BEP/Bestanden Bilge/Instances (Synchromodal transport planning with flexible services Mathematical model and heuristic approach)/Instances/6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="11_7BAE928675DC6F2AE1E85D869446E9E15426D3EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1636DBA-D3A7-4D5E-A4D2-CFC768596AAA}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="11_7BAE928675DC6F2AE1E85D869446E9E15426D3EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E88ED62-CA3C-4912-8F4C-37AB6858B34E}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" tabRatio="773" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -921,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -1326,8 +1326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1731,7 +1731,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K11"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2055,7 +2055,8 @@
         <v>13333333.333333334</v>
       </c>
       <c r="K9" s="2">
-        <v>13333333.333333334</v>
+        <f>444/75</f>
+        <v>5.92</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2119,7 +2120,8 @@
         <v>13333333.333333334</v>
       </c>
       <c r="I11" s="2">
-        <v>13333333.333333334</v>
+        <f>444/75</f>
+        <v>5.92</v>
       </c>
       <c r="J11" s="2">
         <v>13333333.333333334</v>

</xml_diff>